<commit_message>
printing assign asset is added
</commit_message>
<xml_diff>
--- a/FormulariodePrestamosdeEquipo.xlsx
+++ b/FormulariodePrestamosdeEquipo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APM_Setup\htdocs\PhpProject1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qnfeh\OneDrive\문서\NetBeansProjects\PhpProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>MARCA :</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>[onshow.x_desc]</t>
+  </si>
+  <si>
+    <t>[onshow.x_desc]</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
@@ -153,11 +156,11 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>[onshow.x_detail]</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>[onshow.x_in]</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>[onshow.x_detail]</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
 </sst>
@@ -274,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -347,6 +350,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -823,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41:K41"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,54 +866,54 @@
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
       <c r="L6" s="8"/>
     </row>
     <row r="7" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
       <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="L8" s="8"/>
     </row>
     <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
     </row>
     <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
@@ -958,7 +964,7 @@
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
       <c r="D13" s="31" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
@@ -993,7 +999,7 @@
         <v>9</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
@@ -1018,7 +1024,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
@@ -1043,7 +1049,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D22" s="28"/>
       <c r="E22" s="28"/>
@@ -1068,7 +1074,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
@@ -1093,7 +1099,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D26" s="28"/>
       <c r="E26" s="28"/>
@@ -1162,7 +1168,7 @@
         <v>12</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E33" s="28"/>
       <c r="F33" s="28"/>
@@ -1200,7 +1206,7 @@
         <v>26</v>
       </c>
       <c r="D36" s="28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E36" s="28"/>
       <c r="F36" s="28"/>
@@ -1224,15 +1230,13 @@
     </row>
     <row r="38" spans="1:11" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
     </row>
     <row r="39" spans="1:11" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -1263,15 +1267,15 @@
       <c r="K40" s="29"/>
     </row>
     <row r="41" spans="1:11" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="29"/>
-      <c r="J41" s="29"/>
-      <c r="K41" s="29"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="33"/>
     </row>
     <row r="42" spans="1:11" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E42" s="3"/>
@@ -1282,19 +1286,19 @@
       <c r="J42" s="3"/>
     </row>
     <row r="43" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
-      <c r="K43" s="34"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="35"/>
     </row>
     <row r="44" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="27"/>
@@ -1324,7 +1328,7 @@
         <v>4</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D46" s="32"/>
       <c r="E46" s="32"/>
@@ -1341,15 +1345,15 @@
       <c r="B47" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
       <c r="H47" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I47" s="37"/>
-      <c r="J47" s="37"/>
-      <c r="K47" s="37"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="38"/>
+      <c r="K47" s="38"/>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
@@ -1360,22 +1364,24 @@
       <c r="J48" s="7"/>
     </row>
     <row r="49" spans="1:18" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="34" t="s">
+      <c r="A49" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="34"/>
-      <c r="I49" s="34"/>
-      <c r="J49" s="34"/>
-      <c r="K49" s="34"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="35"/>
     </row>
     <row r="50" spans="1:18" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="27"/>
+      <c r="B50" s="27" t="s">
+        <v>33</v>
+      </c>
       <c r="C50" s="27"/>
       <c r="D50" s="27"/>
       <c r="E50" s="27"/>
@@ -1417,15 +1423,15 @@
       <c r="B53" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
       <c r="H53" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I53" s="37"/>
-      <c r="J53" s="37"/>
-      <c r="K53" s="37"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="38"/>
+      <c r="K53" s="38"/>
     </row>
     <row r="54" spans="1:18" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="7"/>
@@ -1471,12 +1477,12 @@
       <c r="R56" s="3"/>
     </row>
     <row r="57" spans="1:18" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B57" s="35"/>
-      <c r="C57" s="35"/>
-      <c r="D57" s="35"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="36"/>
       <c r="G57" s="4" t="s">
         <v>3</v>
       </c>
@@ -1507,7 +1513,7 @@
       <c r="A67" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="36">
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A9:K9"/>
     <mergeCell ref="A7:K7"/>
@@ -1544,7 +1550,6 @@
     <mergeCell ref="C41:K41"/>
     <mergeCell ref="B44:E44"/>
     <mergeCell ref="H44:K44"/>
-    <mergeCell ref="C38:K38"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>